<commit_message>
finished lab_user_data excel sheet and pulling into gui
</commit_message>
<xml_diff>
--- a/Bioreactor Controls/gui_data/lab_user_settings.xlsx
+++ b/Bioreactor Controls/gui_data/lab_user_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmlut\Google Drive\School\Capstone\heart_valve_bioreactor\Bioreactor Controls\gui_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3773E690-F25C-418B-BA12-8344E2FF6740}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AE7D7F-7BDF-44E3-AF80-C3EED85A7DB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49B82CFA-B004-4B79-9632-09EFDC873746}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>Experiment Name</t>
   </si>
@@ -55,16 +55,16 @@
     <t>Single Valve - Systemic</t>
   </si>
   <si>
-    <t>BPM</t>
-  </si>
-  <si>
     <t>Data Frequency (Hz)</t>
   </si>
   <si>
     <t>Save Location</t>
   </si>
   <si>
-    <t>\data\Ted</t>
+    <t>\experiment_data\Ted</t>
+  </si>
+  <si>
+    <t>Time Rest (later bpm)</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,18 +486,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>70</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>50</v>
@@ -508,13 +508,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -524,15 +524,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995A1C14-DF97-437D-8F53-4BCC0959D42F}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.44140625" customWidth="1"/>
   </cols>
@@ -594,13 +594,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>70</v>
-      </c>
-      <c r="C6">
-        <v>70</v>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>